<commit_message>
plotly_test.py - added SQL queries for graph data
</commit_message>
<xml_diff>
--- a/fitness app/exercises_csv/source_exercises.xlsx
+++ b/fitness app/exercises_csv/source_exercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparky\Desktop\CS50\CS50X\finalproject\fitness app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparky\Desktop\CS50\CS50X\finalproject\fitness app\exercises_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B92286-7331-481A-A5DD-33068BE40E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE4C072-88DB-4067-8348-74ADF8047722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StrengthLog Source List" sheetId="1" r:id="rId1"/>
@@ -4450,7 +4450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7D716F-81F1-4EF2-BF6E-9D228E7B52FA}">
   <dimension ref="A1:C242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7058,8 +7058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BC50E2-A4E2-4AEF-A6CB-1C8F1B75A34F}">
   <dimension ref="A1:J336"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>